<commit_message>
Updated 1st May 2024
</commit_message>
<xml_diff>
--- a/resources/resources.xlsx
+++ b/resources/resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaikh Javed\Desktop\github\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA48C33D-7766-478A-BDFC-D5870E8AD60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F92043-3297-4DD7-A44C-85C6A6495E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Skills</t>
   </si>
@@ -115,6 +115,45 @@
   </si>
   <si>
     <t>CN</t>
+  </si>
+  <si>
+    <t>Spark, Databricks</t>
+  </si>
+  <si>
+    <t>Trendytech Ultimate Big Data Masters - Week 3, 4, 5, 6, 7, 8, 9, 10, 11</t>
+  </si>
+  <si>
+    <t>Trendytech Ultimate Big Data Masters - Week 17, 18, 19, 20</t>
+  </si>
+  <si>
+    <t>Trendytech Big Data Masters - Week 9, 10, 11, 12, 13, 14</t>
+  </si>
+  <si>
+    <t>Trendytech Big Data Masters - Week 15, 16, 17</t>
+  </si>
+  <si>
+    <t>Trendytech Ultimate Big Data Masters - Week 26, 27, 28, 29, 30</t>
+  </si>
+  <si>
+    <t>Udemy - Prashant Pandey Stream Processing in Lakehouse course</t>
+  </si>
+  <si>
+    <t>Scholarnest - Apace Spark Performance Tuning course</t>
+  </si>
+  <si>
+    <t>Udemy - Prashant Pandey Master Databricks course</t>
+  </si>
+  <si>
+    <t>Snowflake</t>
+  </si>
+  <si>
+    <t>Flink</t>
+  </si>
+  <si>
+    <t>Azure</t>
+  </si>
+  <si>
+    <t>AWS</t>
   </si>
 </sst>
 </file>
@@ -484,16 +523,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8D9294-542A-46CE-A4A6-2D7BFC4D391B}">
   <dimension ref="C3:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="35.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="57.140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="71.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
@@ -618,6 +658,69 @@
         <v>25</v>
       </c>
     </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C61" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C64" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C81" s="1" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Update 2nd May 2024
</commit_message>
<xml_diff>
--- a/resources/resources.xlsx
+++ b/resources/resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaikh Javed\Desktop\github\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F92043-3297-4DD7-A44C-85C6A6495E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A073330B-710E-4DA5-9C31-07F794C4E940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
   </bookViews>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8D9294-542A-46CE-A4A6-2D7BFC4D391B}">
   <dimension ref="C3:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated 3rd May 2024 1
</commit_message>
<xml_diff>
--- a/resources/resources.xlsx
+++ b/resources/resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaikh Javed\Desktop\github\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A073330B-710E-4DA5-9C31-07F794C4E940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A11B1A-5F29-4A04-B79F-E3209305714F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Skills</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>AWS</t>
+  </si>
+  <si>
+    <t>Number of times revised</t>
+  </si>
+  <si>
+    <t>Trendytech Ultimate Big Data Masters - Week 29</t>
   </si>
 </sst>
 </file>
@@ -521,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8D9294-542A-46CE-A4A6-2D7BFC4D391B}">
-  <dimension ref="C3:D87"/>
+  <dimension ref="C3:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -536,15 +542,18 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
@@ -552,12 +561,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
@@ -565,12 +574,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
@@ -578,12 +587,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
@@ -591,12 +600,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>12</v>
       </c>
@@ -604,144 +613,176 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D28" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D35" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="1" t="s">
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C43" s="1" t="s">
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D44" s="1" t="s">
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D45" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D45" s="1" t="s">
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D46" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D47" s="1" t="s">
+      <c r="E46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D48" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D48" s="1" t="s">
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="1" t="s">
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D50" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D51" s="1" t="s">
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D52" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="1" t="s">
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D53" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="1" t="s">
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C56" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="1" t="s">
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C59" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C61" s="1" t="s">
+    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C62" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C64" s="1" t="s">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81" s="1" t="s">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C82" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C84" s="1" t="s">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C85" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D85" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C87" s="1" t="s">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C88" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D88" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated 6th May 2024
</commit_message>
<xml_diff>
--- a/resources/resources.xlsx
+++ b/resources/resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaikh Javed\Desktop\github\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A11B1A-5F29-4A04-B79F-E3209305714F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D87294-63F5-4FA7-AAC2-841CD2F0EA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Skills</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>Trendytech Ultimate Big Data Masters - Week 29</t>
+  </si>
+  <si>
+    <t>dbt</t>
+  </si>
+  <si>
+    <t>Tableau</t>
   </si>
 </sst>
 </file>
@@ -527,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8D9294-542A-46CE-A4A6-2D7BFC4D391B}">
-  <dimension ref="C3:E88"/>
+  <dimension ref="C3:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -754,35 +760,45 @@
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C62" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C82" s="1" t="s">
+    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C96" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D96" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C85" s="1" t="s">
+    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C99" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D99" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C88" s="1" t="s">
+    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C102" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D102" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated 14th May 2024
</commit_message>
<xml_diff>
--- a/resources/resources.xlsx
+++ b/resources/resources.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaikh Javed\Desktop\github\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B9F9C5-4343-4D81-A4ED-35328E5DA435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD326676-5A6F-4B5D-AE6E-626A24CAF378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="1" r:id="rId1"/>
+    <sheet name="Azure" sheetId="2" r:id="rId2"/>
+    <sheet name="AWS" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Skills</t>
   </si>
@@ -135,15 +137,9 @@
     <t>Trendytech Ultimate Big Data Masters - Week 26, 27, 28, 29, 30</t>
   </si>
   <si>
-    <t>Udemy - Prashant Pandey Stream Processing in Lakehouse course</t>
-  </si>
-  <si>
     <t>Scholarnest - Apace Spark Performance Tuning course</t>
   </si>
   <si>
-    <t>Udemy - Prashant Pandey Master Databricks course</t>
-  </si>
-  <si>
     <t>Snowflake</t>
   </si>
   <si>
@@ -156,9 +152,6 @@
     <t>AWS</t>
   </si>
   <si>
-    <t>Number of times revised</t>
-  </si>
-  <si>
     <t>Trendytech Ultimate Big Data Masters - Week 29</t>
   </si>
   <si>
@@ -166,6 +159,34 @@
   </si>
   <si>
     <t>Tableau</t>
+  </si>
+  <si>
+    <t>Udemy - Kafka for Developers - Data Contracts using Schema Registry 
+https://www.udemy.com/course/kafka-for-developers-data-contracts-using-schema-registry/</t>
+  </si>
+  <si>
+    <t>Udemy - Databricks - Master Azure Databricks for Data Engineers
+https://www.udemy.com/course/master-azure-databricks-for-data-engineers/</t>
+  </si>
+  <si>
+    <t>Udemy - Apache Spark and Databricks - Stream Processing in Lakehouse
+https://www.udemy.com/course/spark-streaming-using-python/</t>
+  </si>
+  <si>
+    <t>Udemy - MongoDB - The Complete Developer's Guide 2024
+https://www.udemy.com/course/mongodb-the-complete-developers-guide/</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Scala</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>ADF</t>
   </si>
 </sst>
 </file>
@@ -213,12 +234,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8D9294-542A-46CE-A4A6-2D7BFC4D391B}">
-  <dimension ref="C3:E102"/>
+  <dimension ref="C3:D115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -548,257 +573,250 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="s">
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D48" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D63" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D66" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C69" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C72" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C75" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C78" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D18" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D35" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D36" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E36" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D37" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E37" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D38" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E38" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D45" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D46" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E46" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D48" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D49" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D50" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D52" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E52" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D53" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C56" s="1" t="s">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C59" s="1" t="s">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C62" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C65" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C68" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C71" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C96" s="1" t="s">
+    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C109" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D109" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C99" s="1" t="s">
+    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C112" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C102" s="1" t="s">
+    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C115" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -806,4 +824,46 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF6CFDA-ACA6-47F4-9A30-D66130C6C307}">
+  <dimension ref="C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="4"/>
+    <col min="3" max="3" width="21.42578125" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4F4BFD-2CBF-4AE9-9242-94BB986F3AAC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated may 21 2024
</commit_message>
<xml_diff>
--- a/resources/resources.xlsx
+++ b/resources/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaikh Javed\Desktop\github\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD326676-5A6F-4B5D-AE6E-626A24CAF378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB179A11-D1F2-472C-A8D5-D027A4FF95EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Skills</t>
   </si>
@@ -95,15 +95,9 @@
     <t>Trendytech Big Data Masters - Week 17</t>
   </si>
   <si>
-    <t>Kafka The Definitive Guide Book</t>
-  </si>
-  <si>
     <t>Important blogs</t>
   </si>
   <si>
-    <t>Knowledge Amplifier youtube channel</t>
-  </si>
-  <si>
     <t>Airflow</t>
   </si>
   <si>
@@ -144,12 +138,6 @@
   </si>
   <si>
     <t>Flink</t>
-  </si>
-  <si>
-    <t>Azure</t>
-  </si>
-  <si>
-    <t>AWS</t>
   </si>
   <si>
     <t>Trendytech Ultimate Big Data Masters - Week 29</t>
@@ -187,6 +175,39 @@
   </si>
   <si>
     <t>ADF</t>
+  </si>
+  <si>
+    <t>Youtube - Knowledge Amplifier channel
+https://www.youtube.com/@KnowledgeAmplifier1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Book - Kafka The Definitive Guide </t>
+  </si>
+  <si>
+    <t>Azure Synapse Analytics</t>
+  </si>
+  <si>
+    <t>ADLS Gen2</t>
+  </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>Trendytech Ultimate Big Data Masters - Week 16</t>
+  </si>
+  <si>
+    <t>Trendytech Ultimate Big Data Masters - Week 21, 22</t>
+  </si>
+  <si>
+    <t>Youtube - WafaStudies
+https://www.youtube.com/playlist?list=PLMWaZteqtEaLTJffbbBzVOv9C0otal1FO</t>
+  </si>
+  <si>
+    <t>Youtube - WafaStudies
+https://www.youtube.com/playlist?list=PLMWaZteqtEaLacN3eS3s8pw2jtwBVb1BH</t>
+  </si>
+  <si>
+    <t>Trendytech Ultimate Big Data Masters - Week 23</t>
   </si>
 </sst>
 </file>
@@ -234,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -244,6 +265,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8D9294-542A-46CE-A4A6-2D7BFC4D391B}">
-  <dimension ref="C3:D115"/>
+  <dimension ref="C3:D116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -583,17 +607,17 @@
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
@@ -682,7 +706,7 @@
         <v>19</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.25">
@@ -695,129 +719,119 @@
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D47" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D48" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D49" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D50" s="1" t="s">
-        <v>24</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D50" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D51" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C54" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C57" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D58" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D59" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D61" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D62" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D63" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D65" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D66" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C69" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C72" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C75" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C78" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C81" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C84" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C109" s="1" t="s">
+    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C110" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C113" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D109" s="1" t="s">
+      <c r="D113" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C116" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C112" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C115" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>27</v>
+      <c r="D116" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -828,21 +842,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF6CFDA-ACA6-47F4-9A30-D66130C6C307}">
-  <dimension ref="C4"/>
+  <dimension ref="C4:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="4"/>
-    <col min="3" max="3" width="21.42578125" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="21.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="57.140625" style="4" customWidth="1"/>
+    <col min="5" max="8" width="21.42578125" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D8" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D9" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -856,12 +907,15 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="3" width="9.140625" style="4"/>
+    <col min="4" max="4" width="28.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="57.140625" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated May 22 2024
</commit_message>
<xml_diff>
--- a/resources/resources.xlsx
+++ b/resources/resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaikh Javed\Desktop\github\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB179A11-D1F2-472C-A8D5-D027A4FF95EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6ADD918-1D60-4DDA-B83D-F92FFD72FBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
   </bookViews>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8D9294-542A-46CE-A4A6-2D7BFC4D391B}">
   <dimension ref="C3:D116"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -845,7 +845,7 @@
   <dimension ref="C4:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated May 25 2024
</commit_message>
<xml_diff>
--- a/resources/resources.xlsx
+++ b/resources/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaikh Javed\Desktop\github\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6ADD918-1D60-4DDA-B83D-F92FFD72FBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB71C503-D97A-4B64-9A8D-5C62CD44D163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>Skills</t>
   </si>
@@ -208,6 +208,13 @@
   </si>
   <si>
     <t>Trendytech Ultimate Big Data Masters - Week 23</t>
+  </si>
+  <si>
+    <t>Youtube -
+https://www.youtube.com/@rajasdataengineering7585</t>
+  </si>
+  <si>
+    <t>S3</t>
   </si>
 </sst>
 </file>
@@ -582,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8D9294-542A-46CE-A4A6-2D7BFC4D391B}">
-  <dimension ref="C3:D116"/>
+  <dimension ref="C3:D118"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -790,47 +797,55 @@
         <v>41</v>
       </c>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" s="1" t="s">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D68" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C71" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72" s="1" t="s">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C74" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75" s="1" t="s">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C77" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78" s="1" t="s">
+    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C80" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C110" s="1" t="s">
+    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C112" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D110" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C113" s="1" t="s">
+    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C115" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C116" s="1" t="s">
+    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C118" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D118" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -844,7 +859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF6CFDA-ACA6-47F4-9A30-D66130C6C307}">
   <dimension ref="C4:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -904,10 +919,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4F4BFD-2CBF-4AE9-9242-94BB986F3AAC}">
-  <dimension ref="A1"/>
+  <dimension ref="D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -917,7 +932,13 @@
     <col min="5" max="5" width="57.140625" style="4" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="4"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="5" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated 30th May 2024
</commit_message>
<xml_diff>
--- a/resources/resources.xlsx
+++ b/resources/resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaikh Javed\Desktop\github\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB71C503-D97A-4B64-9A8D-5C62CD44D163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E692B358-CC5E-4159-85FC-AC7E943FEC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
   <si>
     <t>Skills</t>
   </si>
@@ -215,6 +215,44 @@
   </si>
   <si>
     <t>S3</t>
+  </si>
+  <si>
+    <t>IAM</t>
+  </si>
+  <si>
+    <t>EC2</t>
+  </si>
+  <si>
+    <t>Adrian Cantrill -
+https://learn.cantrill.io/p/aws-certified-solutions-architect-associate-saa-c03</t>
+  </si>
+  <si>
+    <t>Udemy - Data Engineering using AWS Data Analytics
+https://www.udemy.com/course/data-engineering-using-aws-analytics-services/</t>
+  </si>
+  <si>
+    <t>Lambda</t>
+  </si>
+  <si>
+    <t>Glue</t>
+  </si>
+  <si>
+    <t>EMR</t>
+  </si>
+  <si>
+    <t>Athena</t>
+  </si>
+  <si>
+    <t>Kinesis</t>
+  </si>
+  <si>
+    <t>Redshift</t>
+  </si>
+  <si>
+    <t>RDS</t>
+  </si>
+  <si>
+    <t>DynamoDB</t>
   </si>
 </sst>
 </file>
@@ -591,7 +629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8D9294-542A-46CE-A4A6-2D7BFC4D391B}">
   <dimension ref="C3:D118"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
@@ -919,10 +957,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4F4BFD-2CBF-4AE9-9242-94BB986F3AAC}">
-  <dimension ref="D5"/>
+  <dimension ref="D5:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -933,9 +971,94 @@
     <col min="6" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D5" s="4" t="s">
         <v>59</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E6" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E10" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E14" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E18" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="5"/>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 9th June 2024
</commit_message>
<xml_diff>
--- a/resources/resources.xlsx
+++ b/resources/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaikh Javed\Desktop\github\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E692B358-CC5E-4159-85FC-AC7E943FEC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828A1C6D-C6A7-4D13-A946-F797C01218D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="99">
   <si>
     <t>Skills</t>
   </si>
@@ -253,13 +253,96 @@
   </si>
   <si>
     <t>DynamoDB</t>
+  </si>
+  <si>
+    <t>Step Functions</t>
+  </si>
+  <si>
+    <t>API Gateway</t>
+  </si>
+  <si>
+    <t>ELB</t>
+  </si>
+  <si>
+    <t>SNS</t>
+  </si>
+  <si>
+    <t>SQS</t>
+  </si>
+  <si>
+    <t>Backup</t>
+  </si>
+  <si>
+    <t>EBS</t>
+  </si>
+  <si>
+    <t>EFS</t>
+  </si>
+  <si>
+    <t>DMS</t>
+  </si>
+  <si>
+    <t>SCT</t>
+  </si>
+  <si>
+    <t>Snowball</t>
+  </si>
+  <si>
+    <t>Aurora</t>
+  </si>
+  <si>
+    <t>Systems Manager</t>
+  </si>
+  <si>
+    <t>ECS</t>
+  </si>
+  <si>
+    <t>EKS</t>
+  </si>
+  <si>
+    <t>VPC</t>
+  </si>
+  <si>
+    <t>R53</t>
+  </si>
+  <si>
+    <t>AMI</t>
+  </si>
+  <si>
+    <t>KMS</t>
+  </si>
+  <si>
+    <t>CloudTrail</t>
+  </si>
+  <si>
+    <t>Control Tower</t>
+  </si>
+  <si>
+    <t>CloudFormation</t>
+  </si>
+  <si>
+    <t>EventBridge</t>
+  </si>
+  <si>
+    <t>CloudWatch</t>
+  </si>
+  <si>
+    <t>Organizations</t>
+  </si>
+  <si>
+    <t>Youtube - WafaStudies
+https://www.youtube.com/playlist?list=PLMWaZteqtEaIZxPCw_0AO1GsqESq3hZc6</t>
+  </si>
+  <si>
+    <t>Youtube - WafaStudies
+https://www.youtube.com/playlist?list=PLMWaZteqtEaKxRIiTtO7kSKpGVZq2H9uO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,8 +356,22 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,6 +384,16 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -297,10 +404,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -313,8 +422,16 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -629,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8D9294-542A-46CE-A4A6-2D7BFC4D391B}">
   <dimension ref="C3:D118"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71:D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -895,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF6CFDA-ACA6-47F4-9A30-D66130C6C307}">
-  <dimension ref="C4:D15"/>
+  <dimension ref="C4:D17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -945,8 +1062,18 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
+    <row r="13" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D13" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -957,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4F4BFD-2CBF-4AE9-9242-94BB986F3AAC}">
-  <dimension ref="D5:E39"/>
+  <dimension ref="D3:E117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -971,94 +1098,280 @@
     <col min="6" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D5" s="4" t="s">
+    <row r="3" spans="4:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="D3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E3" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="E6" s="5" t="s">
+    <row r="4" spans="4:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E4" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D9" s="4" t="s">
+    <row r="7" spans="4:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="D7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E7" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="E10" s="5" t="s">
+    <row r="8" spans="4:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E8" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D13" s="4" t="s">
+    <row r="11" spans="4:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="D11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E11" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="E14" s="5" t="s">
+    <row r="12" spans="4:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E12" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D17" s="4" t="s">
+    <row r="15" spans="4:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="D15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E15" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="E18" s="5" t="s">
+    <row r="16" spans="4:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E16" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="5"/>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="19" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E20" s="5" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="4" t="s">
-        <v>65</v>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="23" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D24" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D27" s="4" t="s">
+      <c r="E24" s="5"/>
+    </row>
+    <row r="26" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D26" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E27" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="5"/>
+    </row>
+    <row r="30" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D30" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="4" t="s">
+      <c r="E30" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E31" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="5"/>
+    </row>
+    <row r="34" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D34" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="4" t="s">
+      <c r="E34" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E35" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="5"/>
+    </row>
+    <row r="38" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D38" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D39" s="4" t="s">
+      <c r="E38" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D41" s="4" t="s">
         <v>71</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E42" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D45" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D48" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D102" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D105" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D108" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D111" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D114" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="4" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 18th June 2024
</commit_message>
<xml_diff>
--- a/resources/resources.xlsx
+++ b/resources/resources.xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaikh Javed\Desktop\github\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828A1C6D-C6A7-4D13-A946-F797C01218D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88799D35-6DF9-45E2-A6E6-314F9D3FEE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Resources" sheetId="1" r:id="rId1"/>
-    <sheet name="Azure" sheetId="2" r:id="rId2"/>
-    <sheet name="AWS" sheetId="3" r:id="rId3"/>
+    <sheet name="Programming Languages" sheetId="4" r:id="rId1"/>
+    <sheet name="CS Fundamentals" sheetId="6" r:id="rId2"/>
+    <sheet name="Data Engineering" sheetId="1" r:id="rId3"/>
+    <sheet name="Azure" sheetId="2" r:id="rId4"/>
+    <sheet name="AWS" sheetId="3" r:id="rId5"/>
+    <sheet name="DevOps" sheetId="7" r:id="rId6"/>
+    <sheet name="Dev" sheetId="9" r:id="rId7"/>
+    <sheet name="DS" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="107">
   <si>
     <t>Skills</t>
   </si>
@@ -336,13 +341,40 @@
   <si>
     <t>Youtube - WafaStudies
 https://www.youtube.com/playlist?list=PLMWaZteqtEaKxRIiTtO7kSKpGVZq2H9uO</t>
+  </si>
+  <si>
+    <t>Udemy - Snowflake Complete Course for Clearing Interviews
+https://www.udemy.com/course/snowflake-complete-course-for-clearing-interviews/</t>
+  </si>
+  <si>
+    <t>Docker</t>
+  </si>
+  <si>
+    <t>Kubernetes</t>
+  </si>
+  <si>
+    <t>Github Actions</t>
+  </si>
+  <si>
+    <t>Udemy - Master Docker &amp; Kubernetes
+udemy.com/course/master-docker-kubernetes/</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Azure Functions</t>
+  </si>
+  <si>
+    <t>Youtube - WafaStudies
+https://www.youtube.com/playlist?list=PLMWaZteqtEaLRsSynAsaS_aLzDPBUU4CV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,8 +402,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,6 +438,12 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -409,23 +459,25 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -743,266 +795,418 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8D9294-542A-46CE-A4A6-2D7BFC4D391B}">
-  <dimension ref="C3:D118"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A34AC3F-6038-4C18-B742-E0E6F03B2723}">
+  <dimension ref="D4:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71:D80"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="35.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="71.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="35.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="71.42578125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
+    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
+    <row r="5" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
+      <c r="E12" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E19E777B-977A-4837-B5A4-703BBDA46FD5}">
+  <dimension ref="D4:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="35.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="71.28515625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8D9294-542A-46CE-A4A6-2D7BFC4D391B}">
+  <dimension ref="C3:D59"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="35.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="71.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="1" t="s">
+    <row r="6" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="1" t="s">
+    <row r="7" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D22" s="1" t="s">
+    <row r="9" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C25" s="1" t="s">
+    <row r="10" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D11" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D26" s="1" t="s">
+    <row r="12" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C29" s="1" t="s">
+    <row r="13" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D15" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D30" s="1" t="s">
+    <row r="16" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="1" t="s">
+    <row r="17" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D19" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="1" t="s">
+    <row r="20" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D21" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="1" t="s">
+    <row r="22" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D23" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D40" s="1" t="s">
+    <row r="24" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C43" s="1" t="s">
+    <row r="25" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="3:4" s="3" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="3:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D29" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C46" s="1" t="s">
+    <row r="30" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D33" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D37" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D40" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="3:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D42" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+    </row>
+    <row r="47" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D47" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D47" s="1" t="s">
+    <row r="48" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D48" s="3" t="s">
+    <row r="49" spans="3:4" s="3" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D49" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="1" t="s">
+    <row r="50" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D50" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D50" s="3" t="s">
+    <row r="51" spans="3:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D51" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D51" s="1" t="s">
+    <row r="52" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D52" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="1" t="s">
+    <row r="53" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+    </row>
+    <row r="54" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C54" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D59" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D61" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D62" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="63" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D63" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="66" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D66" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D67" s="3"/>
-    </row>
-    <row r="68" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D68" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C71" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77" s="1" t="s">
+    <row r="55" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+    </row>
+    <row r="56" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C80" s="1" t="s">
+    <row r="57" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C112" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C115" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="118" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C118" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>25</v>
-      </c>
+    <row r="59" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1010,71 +1214,87 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF6CFDA-ACA6-47F4-9A30-D66130C6C307}">
-  <dimension ref="C4:D17"/>
+  <dimension ref="C3:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="21.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="57.140625" style="4" customWidth="1"/>
-    <col min="5" max="8" width="21.42578125" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="21.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="57.140625" style="3" customWidth="1"/>
+    <col min="5" max="8" width="21.42578125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="4" t="s">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="4" t="s">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D8" s="5" t="s">
+    <row r="9" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D9" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D9" s="5" t="s">
+    <row r="10" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D10" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="4" t="s">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D13" s="3" t="s">
+    <row r="14" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D14" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D14" s="3" t="s">
+    <row r="15" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D15" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="4" t="s">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C21" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1082,299 +1302,383 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4F4BFD-2CBF-4AE9-9242-94BB986F3AAC}">
-  <dimension ref="D3:E117"/>
+  <dimension ref="D3:E119"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="4"/>
-    <col min="4" max="4" width="28.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="57.140625" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="57.140625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="D3" s="4" t="s">
+    <row r="3" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="E4" s="6" t="s">
+    <row r="6" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E6" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="4:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="D7" s="4" t="s">
+    <row r="9" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E9" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="4:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="E8" s="6" t="s">
+    <row r="10" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E10" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="4:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="D11" s="4" t="s">
+    <row r="13" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E13" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="4:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="E12" s="6" t="s">
+    <row r="14" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E14" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="4:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="D15" s="4" t="s">
+    <row r="17" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D17" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E17" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="4:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="E16" s="7" t="s">
+    <row r="18" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E18" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="5"/>
-    </row>
-    <row r="19" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D19" s="4" t="s">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="21" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D21" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="E20" s="5" t="s">
+    <row r="22" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E22" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="5"/>
-    </row>
-    <row r="23" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D23" s="4" t="s">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="4"/>
+    </row>
+    <row r="25" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D25" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E25" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="5"/>
-    </row>
-    <row r="26" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D26" s="4" t="s">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="4"/>
+    </row>
+    <row r="28" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D28" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E28" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="E27" s="5" t="s">
+    <row r="29" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E29" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E28" s="5"/>
-    </row>
-    <row r="30" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D30" s="4" t="s">
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="4"/>
+    </row>
+    <row r="32" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D32" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E32" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="E31" s="5" t="s">
+    <row r="33" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E33" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E32" s="5"/>
-    </row>
-    <row r="34" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D34" s="4" t="s">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="4"/>
+    </row>
+    <row r="36" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D36" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E36" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="E35" s="5" t="s">
+    <row r="37" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E37" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E36" s="5"/>
-    </row>
-    <row r="38" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D38" s="4" t="s">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="4"/>
+    </row>
+    <row r="40" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D40" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E40" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="D41" s="4" t="s">
+    <row r="43" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="D43" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E43" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="4:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="E42" s="6" t="s">
+    <row r="44" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="E44" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D45" s="4" t="s">
+    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D47" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D48" s="4" t="s">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D51" s="4" t="s">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D54" s="4" t="s">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="4" t="s">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D60" s="4" t="s">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D63" s="4" t="s">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D66" s="4" t="s">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D69" s="4" t="s">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D72" s="4" t="s">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D74" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D75" s="4" t="s">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D77" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D78" s="4" t="s">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D81" s="4" t="s">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D84" s="4" t="s">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D87" s="4" t="s">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D90" s="4" t="s">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D93" s="4" t="s">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D96" s="4" t="s">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D99" s="4" t="s">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D102" s="4" t="s">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D104" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D105" s="4" t="s">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D107" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D108" s="4" t="s">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D110" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D111" s="4" t="s">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D113" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D114" s="4" t="s">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D116" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D117" s="4" t="s">
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D119" s="3" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319F8914-10BC-48C1-969E-C1072B109E10}">
+  <dimension ref="D4:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="35.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="71.42578125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D9" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6724628-5F38-4F22-A085-A5E74E88AD31}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D391BF-C23F-4470-8E1F-EBACAA5D113A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated 26th June 2024
</commit_message>
<xml_diff>
--- a/resources/resources.xlsx
+++ b/resources/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaikh Javed\Desktop\github\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88799D35-6DF9-45E2-A6E6-314F9D3FEE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED02963E-10C0-4E97-AE23-7C47D5D691B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Programming Languages" sheetId="4" r:id="rId1"/>
@@ -459,7 +459,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -473,7 +473,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -918,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8D9294-542A-46CE-A4A6-2D7BFC4D391B}">
   <dimension ref="C3:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -931,7 +930,7 @@
     <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
@@ -939,7 +938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
@@ -947,16 +946,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
@@ -964,16 +963,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D9" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>2</v>
       </c>
@@ -981,20 +980,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1002,20 +993,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D16" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
         <v>12</v>
       </c>
@@ -1023,11 +1006,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
@@ -1035,11 +1018,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
         <v>16</v>
       </c>
@@ -1047,20 +1030,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="3:4" s="3" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C27" s="3" t="s">
         <v>35</v>
       </c>
@@ -1068,11 +1043,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="3:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C29" s="3" t="s">
         <v>19</v>
       </c>
@@ -1080,11 +1055,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C31" s="3" t="s">
         <v>28</v>
       </c>
@@ -1092,59 +1067,59 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D32" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D33" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D35" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D36" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="3:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D37" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D39" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="3:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D40" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="3:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D42" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C45" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C47" s="3" t="s">
         <v>20</v>
       </c>
@@ -1152,59 +1127,59 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D48" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="3:4" s="3" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D49" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D50" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="3:4" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D51" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D52" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
     </row>
-    <row r="54" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C54" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
     </row>
-    <row r="56" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C56" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
     </row>
-    <row r="58" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C58" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="59" spans="3:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
     </row>
@@ -1219,7 +1194,7 @@
   <dimension ref="C3:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1306,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4F4BFD-2CBF-4AE9-9242-94BB986F3AAC}">
   <dimension ref="D3:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E8"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1330,12 +1305,12 @@
       <c r="D5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1343,12 +1318,12 @@
       <c r="D9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="10" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1356,12 +1331,12 @@
       <c r="D13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="14" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1369,12 +1344,12 @@
       <c r="D17" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1473,7 +1448,7 @@
       </c>
     </row>
     <row r="44" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="8" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1612,7 +1587,7 @@
   <dimension ref="D4:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated 29th June 2024 1
</commit_message>
<xml_diff>
--- a/resources/resources.xlsx
+++ b/resources/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaikh Javed\Desktop\github\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED02963E-10C0-4E97-AE23-7C47D5D691B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C403AD-B060-4014-8479-798E83991E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Programming Languages" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="108">
   <si>
     <t>Skills</t>
   </si>
@@ -128,12 +128,6 @@
   </si>
   <si>
     <t>Trendytech Big Data Masters - Week 9, 10, 11, 12, 13, 14</t>
-  </si>
-  <si>
-    <t>Trendytech Big Data Masters - Week 15, 16, 17</t>
-  </si>
-  <si>
-    <t>Trendytech Ultimate Big Data Masters - Week 26, 27, 28, 29, 30</t>
   </si>
   <si>
     <t>Scholarnest - Apace Spark Performance Tuning course</t>
@@ -368,6 +362,16 @@
   <si>
     <t>Youtube - WafaStudies
 https://www.youtube.com/playlist?list=PLMWaZteqtEaLRsSynAsaS_aLzDPBUU4CV</t>
+  </si>
+  <si>
+    <t>Udemy - Apache Airflow | A Real-Time &amp; Hands-On Course on Airflow
+https://www.udemy.com/course/apache-airflow/</t>
+  </si>
+  <si>
+    <t>Trendytech Big Data Masters - Week 15, 16</t>
+  </si>
+  <si>
+    <t>Trendytech Ultimate Big Data Masters - Week 26, 27, 28</t>
   </si>
 </sst>
 </file>
@@ -823,7 +827,7 @@
     </row>
     <row r="6" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -837,7 +841,7 @@
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -851,7 +855,7 @@
     </row>
     <row r="12" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -915,10 +919,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8D9294-542A-46CE-A4A6-2D7BFC4D391B}">
-  <dimension ref="C3:D59"/>
+  <dimension ref="C3:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1037,10 +1041,10 @@
     </row>
     <row r="27" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C27" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
@@ -1052,7 +1056,7 @@
         <v>19</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
@@ -1069,119 +1073,122 @@
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D32" s="3" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D33" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D35" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D37" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D39" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D40" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D42" s="4" t="s">
-        <v>58</v>
+    <row r="38" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D38" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D39" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D41" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C45" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
+      <c r="C46" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C47" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D47" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D48" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D49" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D50" s="3" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D51" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-    </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="3" t="s">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="3:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C57" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-    </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
+      <c r="D57" s="4" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
+      <c r="C59" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C61" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1193,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF6CFDA-ACA6-47F4-9A30-D66130C6C307}">
   <dimension ref="C3:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1209,7 +1216,7 @@
   <sheetData>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>1</v>
@@ -1217,59 +1224,59 @@
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D9" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D10" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D14" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D15" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1281,8 +1288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4F4BFD-2CBF-4AE9-9242-94BB986F3AAC}">
   <dimension ref="D3:E119"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1295,7 +1302,7 @@
   <sheetData>
     <row r="3" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>1</v>
@@ -1303,54 +1310,54 @@
     </row>
     <row r="5" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D5" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="E6" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="E10" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D13" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="E14" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D17" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="E18" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
@@ -1358,15 +1365,15 @@
     </row>
     <row r="21" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D21" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="E22" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.25">
@@ -1374,10 +1381,10 @@
     </row>
     <row r="25" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D25" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.25">
@@ -1385,15 +1392,15 @@
     </row>
     <row r="28" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D28" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="E29" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.25">
@@ -1401,15 +1408,15 @@
     </row>
     <row r="32" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D32" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="E33" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.25">
@@ -1417,15 +1424,15 @@
     </row>
     <row r="36" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D36" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="E37" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.25">
@@ -1433,148 +1440,148 @@
     </row>
     <row r="40" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D40" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="D43" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="4:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="E44" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D47" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D80" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D86" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="89" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D89" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="92" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D92" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="95" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D95" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="98" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D98" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="101" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D101" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="104" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D104" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="107" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D107" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="110" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D110" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D113" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="116" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D116" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="119" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D119" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1587,7 +1594,7 @@
   <dimension ref="D4:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1608,23 +1615,23 @@
     </row>
     <row r="6" spans="4:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D6" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="4:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D9" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="12" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D12" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 29th June 2024
</commit_message>
<xml_diff>
--- a/resources/resources.xlsx
+++ b/resources/resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaikh Javed\Desktop\github\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C403AD-B060-4014-8479-798E83991E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11859C4D-3C48-4AEB-BC59-65546252FC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="5" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Programming Languages" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="109">
   <si>
     <t>Skills</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>Trendytech Ultimate Big Data Masters - Week 26, 27, 28</t>
+  </si>
+  <si>
+    <t>Namaste SQL course</t>
   </si>
 </sst>
 </file>
@@ -802,7 +805,7 @@
   <dimension ref="D4:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -857,7 +860,9 @@
       <c r="D12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>108</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -921,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8D9294-542A-46CE-A4A6-2D7BFC4D391B}">
   <dimension ref="C3:D62"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1200,7 +1205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF6CFDA-ACA6-47F4-9A30-D66130C6C307}">
   <dimension ref="C3:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -1288,7 +1293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4F4BFD-2CBF-4AE9-9242-94BB986F3AAC}">
   <dimension ref="D3:E119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -1593,7 +1598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319F8914-10BC-48C1-969E-C1072B109E10}">
   <dimension ref="D4:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated 5th July 2024
</commit_message>
<xml_diff>
--- a/resources/resources.xlsx
+++ b/resources/resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaikh Javed\Desktop\github\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11859C4D-3C48-4AEB-BC59-65546252FC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E25698-0683-40FF-9C03-326352CF3284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="5" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="2" xr2:uid="{967C0FAC-0701-4A5C-BCCD-F2E3519626CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Programming Languages" sheetId="4" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="DevOps" sheetId="7" r:id="rId6"/>
     <sheet name="Dev" sheetId="9" r:id="rId7"/>
     <sheet name="DS" sheetId="8" r:id="rId8"/>
+    <sheet name="Sys Design" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="112">
   <si>
     <t>Skills</t>
   </si>
@@ -375,6 +376,17 @@
   </si>
   <si>
     <t>Namaste SQL course</t>
+  </si>
+  <si>
+    <t>Trendytech Ultimate Big Data Masters - Week 25</t>
+  </si>
+  <si>
+    <t>Udemy - EssentialSQL: Data Modeling &amp; Relational Data Architecture
+https://www.udemy.com/course/relational-database-design-sql/</t>
+  </si>
+  <si>
+    <t>Udemy - Data Warehouse - The Ultimate Guide
+https://www.udemy.com/course/data-warehouse-the-ultimate-guide/</t>
   </si>
 </sst>
 </file>
@@ -805,7 +817,7 @@
   <dimension ref="D4:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -874,7 +886,7 @@
   <dimension ref="D4:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -926,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8D9294-542A-46CE-A4A6-2D7BFC4D391B}">
   <dimension ref="C3:D62"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1205,7 +1217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF6CFDA-ACA6-47F4-9A30-D66130C6C307}">
   <dimension ref="C3:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -1598,7 +1610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319F8914-10BC-48C1-969E-C1072B109E10}">
   <dimension ref="D4:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1649,7 +1661,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,10 +1674,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D391BF-C23F-4470-8E1F-EBACAA5D113A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9064547E-B519-45C5-ACFF-7482259010BD}">
+  <dimension ref="E4:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="71.42578125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="5:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E8" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="5:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E9" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>